<commit_message>
atualizacao dos graficos e criacao do grafico do protetor
</commit_message>
<xml_diff>
--- a/assets/forerunner_245.xlsx
+++ b/assets/forerunner_245.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,29 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>21:13</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1829</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
atualizacao dos graficos e adicao de uma linha do preco medio
</commit_message>
<xml_diff>
--- a/assets/forerunner_245.xlsx
+++ b/assets/forerunner_245.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -878,6 +878,52 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45211</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>16:08</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1829</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45211</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1829</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
inicio da construcao do dash
</commit_message>
<xml_diff>
--- a/assets/forerunner_245.xlsx
+++ b/assets/forerunner_245.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,6 +947,98 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45215</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>19:33</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45217</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>19:34</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45218</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>21:26</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45220</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1954</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
mudando layout do dash
</commit_message>
<xml_diff>
--- a/assets/forerunner_245.xlsx
+++ b/assets/forerunner_245.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1154,6 +1154,75 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>45228</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>2090</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>20:58</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2090</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2090</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
callbacks para mudar a imagem
</commit_message>
<xml_diff>
--- a/assets/forerunner_245.xlsx
+++ b/assets/forerunner_245.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1315,6 +1315,29 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45235</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11:20</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1819</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
arrumando o grafico de 2 cores
</commit_message>
<xml_diff>
--- a/assets/forerunner_245.xlsx
+++ b/assets/forerunner_245.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1338,6 +1338,52 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45236</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>20:40</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1819</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>20:28</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>amazon</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>preto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>